<commit_message>
Inbox active status indication fixed
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro15/Documents/QuickMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63C6AE9-1029-D94B-8E7E-58C34CEB55F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA852776-BA94-E84D-8CEB-7AAB774F9E3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{35DD9718-AB40-CA45-A8D0-41B6B2CE3BDB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
   <si>
     <t xml:space="preserve"> send complex email with russian subject and body  and attachments (attach throug button and drop)</t>
   </si>
@@ -872,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AFC0D6-220D-4944-BCAA-46D6DFA5B00B}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,7 +886,7 @@
     <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
@@ -899,11 +899,17 @@
       <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="G1" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -917,7 +923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -928,7 +934,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -939,7 +945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -950,7 +956,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -961,7 +967,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -972,7 +978,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -983,7 +989,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -994,7 +1000,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1027,7 +1033,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1060,7 +1066,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
application update with redux engine
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro15/Documents/QuickMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA852776-BA94-E84D-8CEB-7AAB774F9E3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B100BF1-04ED-2342-8828-EF90FCF45A43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{35DD9718-AB40-CA45-A8D0-41B6B2CE3BDB}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28360" windowHeight="17540" xr2:uid="{35DD9718-AB40-CA45-A8D0-41B6B2CE3BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t xml:space="preserve"> send complex email with russian subject and body  and attachments (attach throug button and drop)</t>
   </si>
@@ -213,10 +213,13 @@
     <t>все еще требует sudo пароь nginx после перезапуск uwsgi</t>
   </si>
   <si>
-    <t>SOSO</t>
-  </si>
-  <si>
     <t>safari, VK</t>
+  </si>
+  <si>
+    <t>language switch</t>
+  </si>
+  <si>
+    <t>theme switch</t>
   </si>
 </sst>
 </file>
@@ -269,9 +272,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -279,146 +282,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -576,9 +439,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -616,7 +479,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -722,7 +585,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -872,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AFC0D6-220D-4944-BCAA-46D6DFA5B00B}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,7 +766,7 @@
         <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>35</v>
@@ -917,7 +780,7 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
         <v>61</v>
@@ -975,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -986,7 +849,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -997,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1008,7 +871,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1019,7 +882,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1030,7 +893,7 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1041,7 +904,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1052,7 +915,7 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1063,7 +926,7 @@
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1074,7 +937,7 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1085,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1096,7 +959,7 @@
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1107,7 +970,7 @@
         <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1118,7 +981,7 @@
         <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1129,7 +992,7 @@
         <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1140,7 +1003,7 @@
         <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1151,7 +1014,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1162,7 +1025,7 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1173,7 +1036,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1184,7 +1047,7 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1195,7 +1058,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1206,7 +1069,7 @@
         <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1217,7 +1080,7 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1228,7 +1091,7 @@
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1239,7 +1102,7 @@
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1250,7 +1113,7 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1261,7 +1124,7 @@
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1272,7 +1135,7 @@
         <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1283,7 +1146,7 @@
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
         <v>60</v>
@@ -1297,7 +1160,7 @@
         <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1308,7 +1171,7 @@
         <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1319,7 +1182,7 @@
         <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1330,7 +1193,7 @@
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1341,7 +1204,7 @@
         <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1352,7 +1215,7 @@
         <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1363,7 +1226,7 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1374,7 +1237,7 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1385,7 +1248,7 @@
         <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1396,7 +1259,7 @@
         <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1407,7 +1270,7 @@
         <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1418,7 +1281,7 @@
         <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1429,7 +1292,7 @@
         <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1440,7 +1303,7 @@
         <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1451,7 +1314,7 @@
         <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1462,7 +1325,7 @@
         <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1473,7 +1336,7 @@
         <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1484,7 +1347,7 @@
         <v>32</v>
       </c>
       <c r="C53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -1495,7 +1358,7 @@
         <v>59</v>
       </c>
       <c r="C54" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -1506,63 +1369,85 @@
         <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C136">
-    <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="15" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C13">
-    <cfRule type="containsText" dxfId="28" priority="12" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C15">
-    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="24" priority="8" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",C16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",C22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="7" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",C36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="NOK">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="NOK">
       <formula>NOT(ISERROR(SEARCH("NOK",C49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C49)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>